<commit_message>
Create some additionanal groupings
</commit_message>
<xml_diff>
--- a/data/outputVariables.xlsx
+++ b/data/outputVariables.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/fleminte_staff_vuw_ac_nz/Documents/3 a Res_HRC data/PrevReport/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="348" documentId="13_ncr:1_{66002B5A-1D09-43B0-BE8F-007DBCE076C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9F827392-A1F2-408E-B50A-A3413F4DB995}"/>
+  <xr:revisionPtr revIDLastSave="363" documentId="13_ncr:1_{66002B5A-1D09-43B0-BE8F-007DBCE076C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1C9DD68-B69E-406C-848D-66F24A35238F}"/>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="2100" windowWidth="24390" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
     <sheet name="timeSeries" sheetId="7" r:id="rId2"/>
-    <sheet name="All variables" sheetId="8" r:id="rId3"/>
-    <sheet name="CustomGroup" sheetId="10" r:id="rId4"/>
-    <sheet name="unused time series" sheetId="9" r:id="rId5"/>
+    <sheet name="groupingVariables" sheetId="11" r:id="rId3"/>
+    <sheet name="All variables" sheetId="8" r:id="rId4"/>
+    <sheet name="CustomGroup" sheetId="10" r:id="rId5"/>
+    <sheet name="unused time series" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">variables!$A$1:$F$229</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4396" uniqueCount="1920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4397" uniqueCount="1920">
   <si>
     <t>Emot2</t>
   </si>
@@ -5676,9 +5677,6 @@
     <t>Engaged in vigorous physical activity 4 or more times in the last week</t>
   </si>
   <si>
-    <t>Community</t>
-  </si>
-  <si>
     <t>Helping in Community</t>
   </si>
   <si>
@@ -5800,6 +5798,9 @@
   </si>
   <si>
     <t>Vigorous physical activity  or more times in the past week: Comparisons 2001 - 2019</t>
+  </si>
+  <si>
+    <t>trans</t>
   </si>
 </sst>
 </file>
@@ -6648,8 +6649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
-      <selection activeCell="C277" sqref="C277"/>
+    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
+      <selection activeCell="D272" sqref="D272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8860,7 +8861,9 @@
       <c r="E132" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="F132" s="14"/>
+      <c r="F132" s="14" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D133" s="4"/>
@@ -10779,11 +10782,11 @@
       <c r="D249" s="23"/>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
+      <c r="A250" s="22" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B250" t="s">
         <v>1878</v>
-      </c>
-      <c r="B250" t="s">
-        <v>1879</v>
       </c>
       <c r="C250" t="s">
         <v>1865</v>
@@ -10792,18 +10795,18 @@
         <v>1</v>
       </c>
       <c r="E250" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="F250" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B253" t="s">
         <v>1881</v>
-      </c>
-      <c r="B253" t="s">
-        <v>1882</v>
       </c>
       <c r="C253" t="s">
         <v>371</v>
@@ -10812,18 +10815,18 @@
         <v>1</v>
       </c>
       <c r="E253" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="F253" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B254" s="2" t="s">
         <v>1881</v>
-      </c>
-      <c r="B254" s="2" t="s">
-        <v>1882</v>
       </c>
       <c r="C254" s="2" t="s">
         <v>372</v>
@@ -10832,18 +10835,18 @@
         <v>1</v>
       </c>
       <c r="E254" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="F254" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B255" s="2" t="s">
         <v>1881</v>
-      </c>
-      <c r="B255" s="2" t="s">
-        <v>1882</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>373</v>
@@ -10852,18 +10855,18 @@
         <v>1</v>
       </c>
       <c r="E255" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="F255" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="256" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B256" s="2" t="s">
         <v>1881</v>
-      </c>
-      <c r="B256" s="2" t="s">
-        <v>1882</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>1665</v>
@@ -10872,18 +10875,18 @@
         <v>1</v>
       </c>
       <c r="E256" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="F256" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B257" s="2" t="s">
         <v>1881</v>
-      </c>
-      <c r="B257" s="2" t="s">
-        <v>1882</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>374</v>
@@ -10892,18 +10895,18 @@
         <v>1</v>
       </c>
       <c r="E257" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="F257" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B258" s="2" t="s">
         <v>1881</v>
-      </c>
-      <c r="B258" s="2" t="s">
-        <v>1882</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>1667</v>
@@ -10912,10 +10915,10 @@
         <v>1</v>
       </c>
       <c r="E258" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="F258" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.25">
@@ -10924,10 +10927,10 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B260" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="C260" s="22" t="s">
         <v>1869</v>
@@ -10936,18 +10939,18 @@
         <v>1</v>
       </c>
       <c r="E260" t="s">
+        <v>1889</v>
+      </c>
+      <c r="F260" t="s">
         <v>1890</v>
-      </c>
-      <c r="F260" t="s">
-        <v>1891</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B261" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="C261" s="22" t="s">
         <v>1869</v>
@@ -10956,18 +10959,18 @@
         <v>2</v>
       </c>
       <c r="E261" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="F261" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B262" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="C262" s="22" t="s">
         <v>1869</v>
@@ -10976,18 +10979,18 @@
         <v>3</v>
       </c>
       <c r="E262" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="F262" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B264" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="C264" t="s">
         <v>1151</v>
@@ -10996,18 +10999,18 @@
         <v>1</v>
       </c>
       <c r="E264" t="s">
+        <v>1894</v>
+      </c>
+      <c r="F264" t="s">
         <v>1895</v>
-      </c>
-      <c r="F264" t="s">
-        <v>1896</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B265" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="C265" t="s">
         <v>1151</v>
@@ -11016,18 +11019,18 @@
         <v>2</v>
       </c>
       <c r="E265" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="F265" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B266" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="C266" t="s">
         <v>1151</v>
@@ -11036,18 +11039,18 @@
         <v>3</v>
       </c>
       <c r="E266" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="F266" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B267" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="C267" t="s">
         <v>1151</v>
@@ -11056,78 +11059,78 @@
         <v>4</v>
       </c>
       <c r="E267" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="F267" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B269" t="s">
+        <v>1899</v>
+      </c>
+      <c r="C269" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D269" s="5">
+        <v>0</v>
+      </c>
+      <c r="E269" t="s">
+        <v>1896</v>
+      </c>
+      <c r="F269" t="s">
         <v>1900</v>
-      </c>
-      <c r="C269" t="s">
-        <v>1805</v>
-      </c>
-      <c r="D269" s="5">
-        <v>1</v>
-      </c>
-      <c r="E269" t="s">
-        <v>1897</v>
-      </c>
-      <c r="F269" t="s">
-        <v>1901</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B270" t="s">
-        <v>1900</v>
-      </c>
-      <c r="C270" t="s">
-        <v>1805</v>
+        <v>1899</v>
+      </c>
+      <c r="C270" s="22" t="s">
+        <v>1919</v>
       </c>
       <c r="D270" s="5">
         <v>2</v>
       </c>
       <c r="E270" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="F270" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B271" t="s">
+        <v>1899</v>
+      </c>
+      <c r="C271" s="22" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D271" s="5">
+        <v>1</v>
+      </c>
+      <c r="E271" t="s">
+        <v>1894</v>
+      </c>
+      <c r="F271" t="s">
         <v>1900</v>
-      </c>
-      <c r="C271" t="s">
-        <v>1805</v>
-      </c>
-      <c r="D271" s="5">
-        <v>3</v>
-      </c>
-      <c r="E271" t="s">
-        <v>1895</v>
-      </c>
-      <c r="F271" t="s">
-        <v>1901</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B273" t="s">
         <v>1903</v>
-      </c>
-      <c r="B273" t="s">
-        <v>1904</v>
       </c>
       <c r="C273" t="s">
         <v>354</v>
@@ -11136,18 +11139,18 @@
         <v>1</v>
       </c>
       <c r="E273" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="F273" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B274" t="s">
         <v>1903</v>
-      </c>
-      <c r="B274" t="s">
-        <v>1904</v>
       </c>
       <c r="C274" t="s">
         <v>357</v>
@@ -11156,18 +11159,18 @@
         <v>1</v>
       </c>
       <c r="E274" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="F274" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B275" t="s">
         <v>1903</v>
-      </c>
-      <c r="B275" t="s">
-        <v>1904</v>
       </c>
       <c r="C275" t="s">
         <v>358</v>
@@ -11176,10 +11179,10 @@
         <v>1</v>
       </c>
       <c r="E275" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="F275" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
@@ -11187,7 +11190,7 @@
         <v>551</v>
       </c>
       <c r="B277" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="C277" t="s">
         <v>370</v>
@@ -11199,7 +11202,7 @@
         <v>550</v>
       </c>
       <c r="F277" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
@@ -11207,7 +11210,7 @@
         <v>551</v>
       </c>
       <c r="B278" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="C278" t="s">
         <v>394</v>
@@ -11216,10 +11219,10 @@
         <v>1</v>
       </c>
       <c r="E278" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="F278" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.25">
@@ -11227,7 +11230,7 @@
         <v>551</v>
       </c>
       <c r="B279" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="C279" t="s">
         <v>395</v>
@@ -11236,10 +11239,10 @@
         <v>1</v>
       </c>
       <c r="E279" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="F279" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
@@ -11247,7 +11250,7 @@
         <v>551</v>
       </c>
       <c r="B280" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="C280" t="s">
         <v>392</v>
@@ -11256,10 +11259,10 @@
         <v>1</v>
       </c>
       <c r="E280" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="F280" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
     </row>
   </sheetData>
@@ -12155,10 +12158,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B41" s="30" t="s">
         <v>1916</v>
-      </c>
-      <c r="B41" s="30" t="s">
-        <v>1917</v>
       </c>
       <c r="C41" s="30" t="s">
         <v>1861</v>
@@ -12167,10 +12170,10 @@
         <v>1</v>
       </c>
       <c r="E41" s="30" t="s">
+        <v>1917</v>
+      </c>
+      <c r="F41" s="30" t="s">
         <v>1918</v>
-      </c>
-      <c r="F41" s="30" t="s">
-        <v>1919</v>
       </c>
     </row>
   </sheetData>
@@ -12206,6 +12209,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E33C04A0-A872-4EAA-A318-61F6929E5075}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E93B7FA-B128-4C52-B3FD-D803EA9E6E6C}">
   <dimension ref="A1:F1521"/>
   <sheetViews>
@@ -25946,7 +25963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23D6E65-8B0C-40A2-A858-E67CF09DFD40}">
   <dimension ref="A1:A1509"/>
   <sheetViews>
@@ -33512,7 +33529,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36240CF-41E2-4387-9115-83DEEB4072AE}">
   <dimension ref="A1:F45"/>
   <sheetViews>
@@ -33961,12 +33978,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34193,15 +34207,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABCE2DE6-17B5-4BB3-9252-EC9FC8DD82FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBF97FC-5657-4433-9412-4B0BB8609358}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1ea9f476-e5d7-46f3-a780-376ee5ddd2ee"/>
+    <ds:schemaRef ds:uri="a5d3c314-d92b-413f-ada3-7410c346d515"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -34226,18 +34252,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBF97FC-5657-4433-9412-4B0BB8609358}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABCE2DE6-17B5-4BB3-9252-EC9FC8DD82FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a5d3c314-d92b-413f-ada3-7410c346d515"/>
-    <ds:schemaRef ds:uri="1ea9f476-e5d7-46f3-a780-376ee5ddd2ee"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>